<commit_message>
update tatacara pengambilan data
</commit_message>
<xml_diff>
--- a/data_kecamatan.xlsx
+++ b/data_kecamatan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0. BISMILLAH SKRIPSI\05. Pengolahan\4.4 Dashboard\4.6 Backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0. BISMILLAH SKRIPSI\05. Pengolahan\4.4 Dashboard\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C304D45-58D5-4BDC-9541-CBB02A8C1A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB3A838-0B0E-402C-88AB-195B6BCD4502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,16 +365,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -653,8 +656,8 @@
   </sheetPr>
   <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="I59" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:P79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>